<commit_message>
write file excel analyse bug refacto reader reorg packages
</commit_message>
<xml_diff>
--- a/src/test/resources/personnes.xlsx
+++ b/src/test/resources/personnes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\betton\developpement\github\logiciels\ApiExcel\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{935D28B6-6174-4FA7-8E5B-73170B35DC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A2ED87-396F-4AF3-82BA-4DA150AF6F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57120" yWindow="3615" windowWidth="18900" windowHeight="11055" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -518,8 +518,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,7 +838,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -845,7 +846,7 @@
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="37.28515625" customWidth="1"/>
   </cols>
@@ -860,7 +861,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -880,7 +881,7 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>62860</v>
       </c>
       <c r="E2" t="s">
@@ -900,7 +901,7 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>75250</v>
       </c>
       <c r="E3" t="s">
@@ -920,7 +921,7 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>74252</v>
       </c>
       <c r="E4" t="s">
@@ -940,7 +941,7 @@
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>53319</v>
       </c>
       <c r="E5" t="s">
@@ -960,7 +961,7 @@
       <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>13062</v>
       </c>
       <c r="E6" t="s">
@@ -980,7 +981,7 @@
       <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>45674</v>
       </c>
       <c r="E7" t="s">
@@ -1000,7 +1001,7 @@
       <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>11249</v>
       </c>
       <c r="E8" t="s">
@@ -1020,7 +1021,7 @@
       <c r="C9" t="s">
         <v>43</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>58023</v>
       </c>
       <c r="E9" t="s">
@@ -1040,7 +1041,7 @@
       <c r="C10" t="s">
         <v>48</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>82153</v>
       </c>
       <c r="E10" t="s">
@@ -1060,7 +1061,7 @@
       <c r="C11" t="s">
         <v>53</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>24557</v>
       </c>
       <c r="E11" t="s">
@@ -1080,7 +1081,7 @@
       <c r="C12" t="s">
         <v>58</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>87331</v>
       </c>
       <c r="E12" t="s">
@@ -1100,7 +1101,7 @@
       <c r="C13" t="s">
         <v>63</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>6676</v>
       </c>
       <c r="E13" t="s">
@@ -1120,7 +1121,7 @@
       <c r="C14" t="s">
         <v>68</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>46137</v>
       </c>
       <c r="E14" t="s">
@@ -1140,7 +1141,7 @@
       <c r="C15" t="s">
         <v>73</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>27926</v>
       </c>
       <c r="E15" t="s">
@@ -1160,7 +1161,7 @@
       <c r="C16" t="s">
         <v>78</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>47876</v>
       </c>
       <c r="E16" t="s">
@@ -1180,7 +1181,7 @@
       <c r="C17" t="s">
         <v>83</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>62824</v>
       </c>
       <c r="E17" t="s">
@@ -1200,7 +1201,7 @@
       <c r="C18" t="s">
         <v>88</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>25640</v>
       </c>
       <c r="E18" t="s">
@@ -1220,7 +1221,7 @@
       <c r="C19" t="s">
         <v>93</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>48341</v>
       </c>
       <c r="E19" t="s">
@@ -1240,7 +1241,7 @@
       <c r="C20" t="s">
         <v>98</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>70381</v>
       </c>
       <c r="E20" t="s">
@@ -1260,7 +1261,7 @@
       <c r="C21" t="s">
         <v>102</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>41772</v>
       </c>
       <c r="E21" t="s">
@@ -1280,7 +1281,7 @@
       <c r="C22" t="s">
         <v>107</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>15740</v>
       </c>
       <c r="E22" t="s">
@@ -1300,7 +1301,7 @@
       <c r="C23" t="s">
         <v>112</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>51533</v>
       </c>
       <c r="E23" t="s">
@@ -1320,7 +1321,7 @@
       <c r="C24" t="s">
         <v>117</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>67819</v>
       </c>
       <c r="E24" t="s">
@@ -1340,7 +1341,7 @@
       <c r="C25" t="s">
         <v>122</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>96455</v>
       </c>
       <c r="E25" t="s">
@@ -1360,7 +1361,7 @@
       <c r="C26" t="s">
         <v>127</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>43573</v>
       </c>
       <c r="E26" t="s">
@@ -1380,7 +1381,7 @@
       <c r="C27" t="s">
         <v>132</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>640</v>
       </c>
       <c r="E27" t="s">
@@ -1400,7 +1401,7 @@
       <c r="C28" t="s">
         <v>136</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>65969</v>
       </c>
       <c r="E28" t="s">
@@ -1420,7 +1421,7 @@
       <c r="C29" t="s">
         <v>141</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>21639</v>
       </c>
       <c r="E29" t="s">
@@ -1440,7 +1441,7 @@
       <c r="C30" t="s">
         <v>146</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>67500</v>
       </c>
       <c r="E30" t="s">
@@ -1460,7 +1461,7 @@
       <c r="C31" t="s">
         <v>150</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>21858</v>
       </c>
       <c r="E31" t="s">
@@ -1472,7 +1473,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>